<commit_message>
lun. 11 janv. 2021 14:07:01
</commit_message>
<xml_diff>
--- a/collecte.xlsx
+++ b/collecte.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="collecte" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
   <si>
     <t>kg</t>
   </si>
@@ -27,6 +27,36 @@
   <si>
     <t>05</t>
   </si>
+  <si>
+    <t>Ste</t>
+  </si>
+  <si>
+    <t>Ets</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Lieu</t>
+  </si>
+  <si>
+    <t>Depot</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Qte</t>
+  </si>
+  <si>
+    <t>Un</t>
+  </si>
+  <si>
+    <t>ORI</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +377,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -510,7 +546,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,6 +555,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -856,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -877,35 +919,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2">
-        <v>44166</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2170174</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5010000</v>
-      </c>
-      <c r="H1" s="3">
-        <v>604</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>1</v>
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -919,7 +961,7 @@
         <v>44166</v>
       </c>
       <c r="D2" s="1">
-        <v>2170281</v>
+        <v>2170174</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -931,7 +973,7 @@
         <v>5010000</v>
       </c>
       <c r="H2" s="3">
-        <v>329</v>
+        <v>604</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>0</v>
@@ -951,7 +993,7 @@
         <v>44166</v>
       </c>
       <c r="D3" s="1">
-        <v>2170325</v>
+        <v>2170281</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -963,7 +1005,7 @@
         <v>5010000</v>
       </c>
       <c r="H3" s="3">
-        <v>627</v>
+        <v>329</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>0</v>
@@ -983,7 +1025,7 @@
         <v>44166</v>
       </c>
       <c r="D4" s="1">
-        <v>2170323</v>
+        <v>2170325</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
@@ -995,7 +1037,7 @@
         <v>5010000</v>
       </c>
       <c r="H4" s="3">
-        <v>804</v>
+        <v>627</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>0</v>
@@ -1015,7 +1057,7 @@
         <v>44166</v>
       </c>
       <c r="D5" s="1">
-        <v>2170074</v>
+        <v>2170323</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>2</v>
@@ -1027,7 +1069,7 @@
         <v>5010000</v>
       </c>
       <c r="H5" s="3">
-        <v>151</v>
+        <v>804</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>0</v>
@@ -1047,7 +1089,7 @@
         <v>44166</v>
       </c>
       <c r="D6" s="1">
-        <v>2170308</v>
+        <v>2170074</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>2</v>
@@ -1059,7 +1101,7 @@
         <v>5010000</v>
       </c>
       <c r="H6" s="3">
-        <v>602</v>
+        <v>151</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>0</v>
@@ -1079,7 +1121,7 @@
         <v>44166</v>
       </c>
       <c r="D7" s="1">
-        <v>2170198</v>
+        <v>2170308</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>2</v>
@@ -1091,7 +1133,7 @@
         <v>5010000</v>
       </c>
       <c r="H7" s="3">
-        <v>1061</v>
+        <v>602</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>0</v>
@@ -1111,7 +1153,7 @@
         <v>44166</v>
       </c>
       <c r="D8" s="1">
-        <v>2170073</v>
+        <v>2170198</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>2</v>
@@ -1123,7 +1165,7 @@
         <v>5010000</v>
       </c>
       <c r="H8" s="3">
-        <v>315</v>
+        <v>1061</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>0</v>
@@ -1143,7 +1185,7 @@
         <v>44166</v>
       </c>
       <c r="D9" s="1">
-        <v>2170040</v>
+        <v>2170073</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>2</v>
@@ -1155,7 +1197,7 @@
         <v>5010000</v>
       </c>
       <c r="H9" s="3">
-        <v>128</v>
+        <v>315</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>0</v>
@@ -1175,7 +1217,7 @@
         <v>44166</v>
       </c>
       <c r="D10" s="1">
-        <v>2170138</v>
+        <v>2170040</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>2</v>
@@ -1187,7 +1229,7 @@
         <v>5010000</v>
       </c>
       <c r="H10" s="3">
-        <v>794</v>
+        <v>128</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>0</v>
@@ -1207,7 +1249,7 @@
         <v>44166</v>
       </c>
       <c r="D11" s="1">
-        <v>2170022</v>
+        <v>2170138</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>2</v>
@@ -1219,7 +1261,7 @@
         <v>5010000</v>
       </c>
       <c r="H11" s="3">
-        <v>175</v>
+        <v>794</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>0</v>
@@ -1239,7 +1281,7 @@
         <v>44166</v>
       </c>
       <c r="D12" s="1">
-        <v>2170306</v>
+        <v>2170022</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>2</v>
@@ -1251,7 +1293,7 @@
         <v>5010000</v>
       </c>
       <c r="H12" s="3">
-        <v>717</v>
+        <v>175</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>0</v>
@@ -1271,7 +1313,7 @@
         <v>44166</v>
       </c>
       <c r="D13" s="1">
-        <v>2170139</v>
+        <v>2170306</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>2</v>
@@ -1283,7 +1325,7 @@
         <v>5010000</v>
       </c>
       <c r="H13" s="3">
-        <v>375</v>
+        <v>717</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>0</v>
@@ -1303,7 +1345,7 @@
         <v>44166</v>
       </c>
       <c r="D14" s="1">
-        <v>2170200</v>
+        <v>2170139</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
@@ -1315,7 +1357,7 @@
         <v>5010000</v>
       </c>
       <c r="H14" s="3">
-        <v>603</v>
+        <v>375</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>0</v>
@@ -1335,7 +1377,7 @@
         <v>44166</v>
       </c>
       <c r="D15" s="1">
-        <v>2170346</v>
+        <v>2170200</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>2</v>
@@ -1347,12 +1389,44 @@
         <v>5010000</v>
       </c>
       <c r="H15" s="3">
-        <v>1200</v>
+        <v>603</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44166</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2170346</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5010000</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1200</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>